<commit_message>
chore: update based on 1c56b2f
</commit_message>
<xml_diff>
--- a/checklist/WSTG-Checklist_v4.2.xlsx
+++ b/checklist/WSTG-Checklist_v4.2.xlsx
@@ -607,8 +607,8 @@
     <t xml:space="preserve">Testing for Browser Cache Weaknesses</t>
   </si>
   <si>
-    <t xml:space="preserve">- On disk or in memory, where it might be retrieved after intended use.
-- In such a way that using the Back button may allow a user (or attacker) to return to a previously displayed screen.</t>
+    <t xml:space="preserve">- Review if the application stores sensitive information on the client side.
+- Review if access can occur without authorization.</t>
   </si>
   <si>
     <t xml:space="preserve">WSTG-ATHN-07</t>
@@ -1903,7 +1903,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="57">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1998,26 +1998,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -2206,7 +2186,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="00FFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2216,7 +2196,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="00FFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2226,7 +2206,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="00FFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2236,7 +2216,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="00FFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2246,7 +2226,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="00FFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2256,7 +2236,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="00FFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2463,11 +2443,11 @@
   </sheetPr>
   <dimension ref="A1:Y1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A34" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C44" activeCellId="0" sqref="C44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="51.29"/>
@@ -3256,7 +3236,7 @@
       <c r="B42" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="C42" s="22" t="s">
+      <c r="C42" s="23" t="s">
         <v>104</v>
       </c>
       <c r="D42" s="12" t="s">
@@ -4049,11 +4029,11 @@
       <c r="X81" s="3"/>
       <c r="Y81" s="3"/>
     </row>
-    <row r="82" s="28" customFormat="true" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A82" s="24" t="s">
+    <row r="82" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A82" s="9" t="s">
         <v>206</v>
       </c>
-      <c r="B82" s="25" t="s">
+      <c r="B82" s="16" t="s">
         <v>207</v>
       </c>
       <c r="C82" s="11" t="s">
@@ -4062,27 +4042,27 @@
       <c r="D82" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="E82" s="26"/>
-      <c r="F82" s="27"/>
-      <c r="G82" s="27"/>
-      <c r="H82" s="27"/>
-      <c r="I82" s="27"/>
-      <c r="J82" s="27"/>
-      <c r="K82" s="27"/>
-      <c r="L82" s="27"/>
-      <c r="M82" s="27"/>
-      <c r="N82" s="27"/>
-      <c r="O82" s="27"/>
-      <c r="P82" s="27"/>
-      <c r="Q82" s="27"/>
-      <c r="R82" s="27"/>
-      <c r="S82" s="27"/>
-      <c r="T82" s="27"/>
-      <c r="U82" s="27"/>
-      <c r="V82" s="27"/>
-      <c r="W82" s="27"/>
-      <c r="X82" s="27"/>
-      <c r="Y82" s="27"/>
+      <c r="E82" s="18"/>
+      <c r="F82" s="3"/>
+      <c r="G82" s="3"/>
+      <c r="H82" s="3"/>
+      <c r="I82" s="3"/>
+      <c r="J82" s="3"/>
+      <c r="K82" s="3"/>
+      <c r="L82" s="3"/>
+      <c r="M82" s="3"/>
+      <c r="N82" s="3"/>
+      <c r="O82" s="3"/>
+      <c r="P82" s="3"/>
+      <c r="Q82" s="3"/>
+      <c r="R82" s="3"/>
+      <c r="S82" s="3"/>
+      <c r="T82" s="3"/>
+      <c r="U82" s="3"/>
+      <c r="V82" s="3"/>
+      <c r="W82" s="3"/>
+      <c r="X82" s="3"/>
+      <c r="Y82" s="3"/>
     </row>
     <row r="83" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="9" t="s">
@@ -4157,7 +4137,7 @@
     <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="8"/>
       <c r="B85" s="19"/>
-      <c r="C85" s="29"/>
+      <c r="C85" s="24"/>
       <c r="D85" s="21"/>
       <c r="E85" s="3"/>
       <c r="F85" s="8"/>
@@ -4260,7 +4240,7 @@
       <c r="B88" s="16" t="s">
         <v>220</v>
       </c>
-      <c r="C88" s="30"/>
+      <c r="C88" s="25"/>
       <c r="D88" s="12" t="s">
         <v>9</v>
       </c>
@@ -4393,7 +4373,7 @@
     <row r="95" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="19"/>
       <c r="B95" s="19"/>
-      <c r="C95" s="29"/>
+      <c r="C95" s="24"/>
       <c r="D95" s="21"/>
       <c r="E95" s="3"/>
     </row>
@@ -6611,10 +6591,10 @@
   <dimension ref="A1:J1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D8 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.71"/>
@@ -6629,62 +6609,62 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="26" t="s">
         <v>309</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="26" t="s">
         <v>310</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="26" t="s">
         <v>311</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="26" t="s">
         <v>312</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="26" t="s">
         <v>313</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="26" t="s">
         <v>314</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="G1" s="26" t="s">
         <v>315</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="H1" s="26" t="s">
         <v>316</v>
       </c>
-      <c r="I1" s="31" t="s">
+      <c r="I1" s="26" t="s">
         <v>317</v>
       </c>
-      <c r="J1" s="32" t="s">
+      <c r="J1" s="27" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="33" t="n">
+      <c r="A2" s="28" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="28" t="s">
         <v>319</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="28" t="s">
         <v>170</v>
       </c>
-      <c r="D2" s="33" t="s">
+      <c r="D2" s="28" t="s">
         <v>320</v>
       </c>
-      <c r="E2" s="33" t="s">
+      <c r="E2" s="28" t="s">
         <v>321</v>
       </c>
-      <c r="F2" s="33" t="s">
+      <c r="F2" s="28" t="s">
         <v>322</v>
       </c>
-      <c r="G2" s="34" t="s">
+      <c r="G2" s="29" t="s">
         <v>321</v>
       </c>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33" t="s">
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28" t="s">
         <v>323</v>
       </c>
     </row>
@@ -8182,13 +8162,13 @@
   <dimension ref="A1:H1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D8 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="14.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="14.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="42.71"/>
@@ -8196,60 +8176,60 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="30" t="s">
         <v>324</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="31" t="s">
         <v>325</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="36" t="s">
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="31" t="s">
         <v>326</v>
       </c>
-      <c r="G3" s="36"/>
+      <c r="G3" s="31"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="33" t="s">
         <v>327</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="38" t="s">
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="33" t="s">
         <v>328</v>
       </c>
-      <c r="G4" s="38"/>
+      <c r="G4" s="33"/>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="40" t="s">
+      <c r="A5" s="35" t="s">
         <v>329</v>
       </c>
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="36" t="s">
         <v>330</v>
       </c>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="42" t="n">
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
+      <c r="E5" s="37" t="n">
         <f aca="false">VLOOKUP(B5,References!A2:B8,2,0)</f>
         <v>3</v>
       </c>
-      <c r="F5" s="40" t="s">
+      <c r="F5" s="35" t="s">
         <v>331</v>
       </c>
-      <c r="G5" s="43" t="s">
+      <c r="G5" s="38" t="s">
         <v>332</v>
       </c>
       <c r="H5" s="19" t="n">
@@ -8258,22 +8238,22 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="40" t="s">
+      <c r="A6" s="35" t="s">
         <v>333</v>
       </c>
-      <c r="B6" s="44" t="s">
+      <c r="B6" s="39" t="s">
         <v>334</v>
       </c>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="42" t="n">
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="37" t="n">
         <f aca="false">VLOOKUP(B6,References!C2:D6,2,0)</f>
         <v>4</v>
       </c>
-      <c r="F6" s="40" t="s">
+      <c r="F6" s="35" t="s">
         <v>335</v>
       </c>
-      <c r="G6" s="43" t="s">
+      <c r="G6" s="38" t="s">
         <v>336</v>
       </c>
       <c r="H6" s="19" t="n">
@@ -8282,22 +8262,22 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="40" t="s">
+      <c r="A7" s="35" t="s">
         <v>337</v>
       </c>
-      <c r="B7" s="44" t="s">
+      <c r="B7" s="39" t="s">
         <v>338</v>
       </c>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="42" t="n">
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="37" t="n">
         <f aca="false">VLOOKUP(B7,References!E2:F6,2,0)</f>
         <v>0</v>
       </c>
-      <c r="F7" s="40" t="s">
+      <c r="F7" s="35" t="s">
         <v>339</v>
       </c>
-      <c r="G7" s="43" t="s">
+      <c r="G7" s="38" t="s">
         <v>340</v>
       </c>
       <c r="H7" s="19" t="n">
@@ -8306,22 +8286,22 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="40" t="s">
+      <c r="A8" s="35" t="s">
         <v>341</v>
       </c>
-      <c r="B8" s="44" t="s">
+      <c r="B8" s="39" t="s">
         <v>342</v>
       </c>
-      <c r="C8" s="44"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="42" t="n">
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
+      <c r="E8" s="37" t="n">
         <f aca="false">VLOOKUP(B8,References!G3:H8,2,0)</f>
         <v>2</v>
       </c>
-      <c r="F8" s="40" t="s">
+      <c r="F8" s="35" t="s">
         <v>343</v>
       </c>
-      <c r="G8" s="43" t="s">
+      <c r="G8" s="38" t="s">
         <v>344</v>
       </c>
       <c r="H8" s="19" t="n">
@@ -8330,46 +8310,46 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="40"/>
-      <c r="B9" s="43"/>
-      <c r="C9" s="43"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="43"/>
+      <c r="A9" s="35"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="35"/>
+      <c r="G9" s="38"/>
       <c r="H9" s="19"/>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="33" t="s">
         <v>345</v>
       </c>
-      <c r="B10" s="38"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="38" t="s">
+      <c r="B10" s="33"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="33" t="s">
         <v>346</v>
       </c>
-      <c r="G10" s="38"/>
-      <c r="H10" s="39"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="34"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="40" t="s">
+      <c r="A11" s="35" t="s">
         <v>347</v>
       </c>
-      <c r="B11" s="41" t="s">
+      <c r="B11" s="36" t="s">
         <v>348</v>
       </c>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="42" t="n">
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="37" t="n">
         <f aca="false">VLOOKUP(B11,References!I2:J7,2,0)</f>
         <v>1</v>
       </c>
-      <c r="F11" s="40" t="s">
+      <c r="F11" s="35" t="s">
         <v>349</v>
       </c>
-      <c r="G11" s="43" t="s">
+      <c r="G11" s="38" t="s">
         <v>350</v>
       </c>
       <c r="H11" s="19" t="n">
@@ -8378,22 +8358,22 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="40" t="s">
+      <c r="A12" s="35" t="s">
         <v>351</v>
       </c>
-      <c r="B12" s="41" t="s">
+      <c r="B12" s="36" t="s">
         <v>352</v>
       </c>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="42" t="n">
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="37" t="n">
         <f aca="false">VLOOKUP(B12,References!K$2:L$7,2,0)</f>
         <v>5</v>
       </c>
-      <c r="F12" s="40" t="s">
+      <c r="F12" s="35" t="s">
         <v>353</v>
       </c>
-      <c r="G12" s="43" t="s">
+      <c r="G12" s="38" t="s">
         <v>354</v>
       </c>
       <c r="H12" s="19" t="n">
@@ -8402,22 +8382,22 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="40" t="s">
+      <c r="A13" s="35" t="s">
         <v>355</v>
       </c>
-      <c r="B13" s="41" t="s">
+      <c r="B13" s="36" t="s">
         <v>356</v>
       </c>
-      <c r="C13" s="41"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="42" t="n">
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="37" t="n">
         <f aca="false">VLOOKUP(B13,References!M$2:N$7,2,0)</f>
         <v>4</v>
       </c>
-      <c r="F13" s="40" t="s">
+      <c r="F13" s="35" t="s">
         <v>357</v>
       </c>
-      <c r="G13" s="43" t="s">
+      <c r="G13" s="38" t="s">
         <v>358</v>
       </c>
       <c r="H13" s="19" t="n">
@@ -8426,22 +8406,22 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="40" t="s">
+      <c r="A14" s="35" t="s">
         <v>359</v>
       </c>
-      <c r="B14" s="41" t="s">
+      <c r="B14" s="36" t="s">
         <v>360</v>
       </c>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="42" t="n">
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="37" t="n">
         <f aca="false">VLOOKUP(B14,References!O$2:P$7,2,0)</f>
         <v>3</v>
       </c>
-      <c r="F14" s="40" t="s">
+      <c r="F14" s="35" t="s">
         <v>361</v>
       </c>
-      <c r="G14" s="43" t="s">
+      <c r="G14" s="38" t="s">
         <v>362</v>
       </c>
       <c r="H14" s="19" t="n">
@@ -8450,128 +8430,128 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="E15" s="40"/>
+      <c r="E15" s="35"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="45" t="s">
+      <c r="A16" s="40" t="s">
         <v>363</v>
       </c>
-      <c r="B16" s="46" t="n">
+      <c r="B16" s="41" t="n">
         <f aca="false">IFERROR(AVERAGE(E5:E8,E11:E14),"All factors require a selection.")</f>
         <v>2.75</v>
       </c>
-      <c r="C16" s="46"/>
-      <c r="D16" s="46"/>
-      <c r="E16" s="40"/>
-      <c r="F16" s="47" t="s">
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="42" t="s">
         <v>364</v>
       </c>
-      <c r="G16" s="46" t="n">
+      <c r="G16" s="41" t="n">
         <f aca="false">IFERROR(AVERAGE(H5:H8,H11:H14),"All factors require a selection.")</f>
         <v>3.375</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="45"/>
-      <c r="B17" s="46"/>
-      <c r="C17" s="46"/>
-      <c r="D17" s="46"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="47"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="41"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="42"/>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B20" s="48" t="s">
+      <c r="B20" s="43" t="s">
         <v>365</v>
       </c>
-      <c r="C20" s="48"/>
-      <c r="D20" s="48"/>
-      <c r="E20" s="49" t="str">
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="44" t="str">
         <f aca="false">IFERROR(IF(AND($B$16&lt;3,$G$16&lt;3),"Note",IF(OR(AND($B$16&lt;3,$G$16&gt;=3,$G$16&lt;6),AND($B$16&gt;=3,$B$16&lt;6,$G$16&lt;3)),"Low",IF(OR(AND($B16&lt;3,$G16&gt;=6),AND($B16&gt;=3,$B16&lt;6,$G16&gt;=3,$G16&lt;6),AND($B16&gt;=6,$G16&lt;3)),"MODERATE",IF(OR(AND($B16&gt;=6,$B16&gt;=3,$G16&lt;6),AND($B16&gt;=3,$B16&lt;6,$G16&gt;6)),"High","Critical")))),"Note")</f>
         <v>Low</v>
       </c>
-      <c r="F20" s="49"/>
-      <c r="G20" s="50"/>
+      <c r="F20" s="44"/>
+      <c r="G20" s="45"/>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B22" s="51" t="s">
+      <c r="B22" s="46" t="s">
         <v>313</v>
       </c>
-      <c r="C22" s="51"/>
-      <c r="D22" s="51"/>
+      <c r="C22" s="46"/>
+      <c r="D22" s="46"/>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="52" t="s">
+      <c r="A23" s="47" t="s">
         <v>314</v>
       </c>
-      <c r="B23" s="53" t="str">
+      <c r="B23" s="48" t="str">
         <f aca="false">IF($G16&lt;3,"-&gt;Low&lt;-","Low")</f>
         <v>Low</v>
       </c>
-      <c r="C23" s="53" t="str">
+      <c r="C23" s="48" t="str">
         <f aca="false">IF(AND($G16&gt;=3,$G16&lt;6),"-&gt;Moderate&lt;-","Moderate")</f>
         <v>-&gt;Moderate&lt;-</v>
       </c>
-      <c r="D23" s="53" t="str">
+      <c r="D23" s="48" t="str">
         <f aca="false">IF($G16&gt;=6,"-&gt;High&lt;-","High")</f>
         <v>High</v>
       </c>
       <c r="F23" s="3"/>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="54" t="str">
+      <c r="A24" s="49" t="str">
         <f aca="false">IF($B16&lt;3,"-&gt;Low&lt;-","Low")</f>
         <v>-&gt;Low&lt;-</v>
       </c>
-      <c r="B24" s="55" t="str">
+      <c r="B24" s="50" t="str">
         <f aca="false">IF(AND($B$16&lt;3,$G$16&lt;3),"-&gt;Note&lt;-","Note")</f>
         <v>Note</v>
       </c>
-      <c r="C24" s="56" t="str">
+      <c r="C24" s="51" t="str">
         <f aca="false">IF(AND($B$16&lt;3,$G$16&gt;=3,$G$16&lt;6),"-&gt;Low&lt;-","Low")</f>
         <v>-&gt;Low&lt;-</v>
       </c>
-      <c r="D24" s="57" t="str">
+      <c r="D24" s="52" t="str">
         <f aca="false">IF(AND($B16&lt;3,$G16&gt;=6),"-&gt;Moderate&lt;-","Moderate")</f>
         <v>Moderate</v>
       </c>
-      <c r="F24" s="58"/>
+      <c r="F24" s="53"/>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="54" t="str">
+      <c r="A25" s="49" t="str">
         <f aca="false">IF(AND($B16&gt;=3,$B16&lt;6),"-&gt;Moderate&lt;-","Moderate")</f>
         <v>Moderate</v>
       </c>
-      <c r="B25" s="56" t="str">
+      <c r="B25" s="51" t="str">
         <f aca="false">IF(AND($B$16&gt;=3,$B$16&lt;6,$G$16&lt;3),"-&gt;Low&lt;-","Low")</f>
         <v>Low</v>
       </c>
-      <c r="C25" s="57" t="str">
+      <c r="C25" s="52" t="str">
         <f aca="false">IF(AND($B16&gt;=3,$B16&lt;6,$G16&gt;=3,$G16&lt;6),"-&gt;Moderate&lt;-","Moderate")</f>
         <v>Moderate</v>
       </c>
-      <c r="D25" s="59" t="str">
+      <c r="D25" s="54" t="str">
         <f aca="false">IF(AND($B16&gt;=3,$B16&lt;6,$G16&gt;6),"-&gt;High&lt;-","High")</f>
         <v>High</v>
       </c>
-      <c r="F25" s="58"/>
+      <c r="F25" s="53"/>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="54" t="str">
+      <c r="A26" s="49" t="str">
         <f aca="false">IF($B16&gt;=6,"-&gt;High&lt;-","High")</f>
         <v>High</v>
       </c>
-      <c r="B26" s="57" t="str">
+      <c r="B26" s="52" t="str">
         <f aca="false">IF(AND($B16&gt;=6,$G16&lt;3),"-&gt;Moderate&lt;-","Moderate")</f>
         <v>Moderate</v>
       </c>
-      <c r="C26" s="59" t="str">
+      <c r="C26" s="54" t="str">
         <f aca="false">IF(AND($B16&gt;=6,$B16&gt;=3,$G16&lt;6),"-&gt;High&lt;-","High")</f>
         <v>High</v>
       </c>
-      <c r="D26" s="60" t="str">
+      <c r="D26" s="55" t="str">
         <f aca="false">IF(AND($B$16&gt;=6,$G$16&gt;=6),"-&gt;Critical&lt;-","Critical")</f>
         <v>Critical</v>
       </c>
@@ -9715,10 +9695,10 @@
   <dimension ref="A1:P1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D8 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="2"/>
@@ -9739,35 +9719,35 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="56" t="s">
         <v>329</v>
       </c>
       <c r="B1" s="19"/>
-      <c r="C1" s="61" t="s">
+      <c r="C1" s="56" t="s">
         <v>333</v>
       </c>
       <c r="D1" s="19"/>
-      <c r="E1" s="61" t="s">
+      <c r="E1" s="56" t="s">
         <v>337</v>
       </c>
       <c r="F1" s="19"/>
-      <c r="G1" s="61" t="s">
+      <c r="G1" s="56" t="s">
         <v>341</v>
       </c>
       <c r="H1" s="19"/>
-      <c r="I1" s="61" t="s">
+      <c r="I1" s="56" t="s">
         <v>347</v>
       </c>
       <c r="J1" s="19"/>
-      <c r="K1" s="61" t="s">
+      <c r="K1" s="56" t="s">
         <v>351</v>
       </c>
       <c r="L1" s="19"/>
-      <c r="M1" s="61" t="s">
+      <c r="M1" s="56" t="s">
         <v>355</v>
       </c>
       <c r="N1" s="19"/>
-      <c r="O1" s="61" t="s">
+      <c r="O1" s="56" t="s">
         <v>359</v>
       </c>
       <c r="P1" s="19"/>
@@ -10092,38 +10072,38 @@
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="61" t="s">
+      <c r="A10" s="56" t="s">
         <v>331</v>
       </c>
-      <c r="B10" s="61"/>
-      <c r="C10" s="61" t="s">
+      <c r="B10" s="56"/>
+      <c r="C10" s="56" t="s">
         <v>335</v>
       </c>
-      <c r="D10" s="61"/>
-      <c r="E10" s="61" t="s">
+      <c r="D10" s="56"/>
+      <c r="E10" s="56" t="s">
         <v>339</v>
       </c>
-      <c r="F10" s="61"/>
-      <c r="G10" s="61" t="s">
+      <c r="F10" s="56"/>
+      <c r="G10" s="56" t="s">
         <v>343</v>
       </c>
-      <c r="H10" s="61"/>
-      <c r="I10" s="61" t="s">
+      <c r="H10" s="56"/>
+      <c r="I10" s="56" t="s">
         <v>349</v>
       </c>
-      <c r="J10" s="61"/>
-      <c r="K10" s="61" t="s">
+      <c r="J10" s="56"/>
+      <c r="K10" s="56" t="s">
         <v>353</v>
       </c>
-      <c r="L10" s="61"/>
-      <c r="M10" s="61" t="s">
+      <c r="L10" s="56"/>
+      <c r="M10" s="56" t="s">
         <v>357</v>
       </c>
-      <c r="N10" s="61"/>
-      <c r="O10" s="61" t="s">
+      <c r="N10" s="56"/>
+      <c r="O10" s="56" t="s">
         <v>361</v>
       </c>
-      <c r="P10" s="52"/>
+      <c r="P10" s="47"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="19" t="s">
@@ -10271,7 +10251,7 @@
       <c r="O13" s="19" t="s">
         <v>362</v>
       </c>
-      <c r="P13" s="40" t="n">
+      <c r="P13" s="35" t="n">
         <v>3</v>
       </c>
     </row>
@@ -10321,7 +10301,7 @@
       <c r="O14" s="19" t="s">
         <v>400</v>
       </c>
-      <c r="P14" s="40" t="n">
+      <c r="P14" s="35" t="n">
         <v>5</v>
       </c>
     </row>
@@ -10371,7 +10351,7 @@
       <c r="O15" s="19" t="s">
         <v>408</v>
       </c>
-      <c r="P15" s="40" t="n">
+      <c r="P15" s="35" t="n">
         <v>7</v>
       </c>
     </row>
@@ -10413,7 +10393,7 @@
       <c r="O16" s="19" t="s">
         <v>414</v>
       </c>
-      <c r="P16" s="40" t="n">
+      <c r="P16" s="35" t="n">
         <v>9</v>
       </c>
     </row>

</xml_diff>